<commit_message>
BD 1th sem homework fix
</commit_message>
<xml_diff>
--- a/GB/4.Module Data Base/Seminar 1 Homework .xlsx
+++ b/GB/4.Module Data Base/Seminar 1 Homework .xlsx
@@ -28,91 +28,91 @@
     <t xml:space="preserve">ID Записи</t>
   </si>
   <si>
+    <t xml:space="preserve">ID Автобуса</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID Смены</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID Маршрута</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID Водителя</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID Кондуктор</t>
+  </si>
+  <si>
     <t xml:space="preserve">Автобус</t>
   </si>
   <si>
     <t xml:space="preserve">Смена</t>
   </si>
   <si>
+    <t xml:space="preserve">Водитель</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Номер</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID Модели</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Время</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ФИО</t>
+  </si>
+  <si>
+    <t xml:space="preserve">АВ2453</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06:00-12:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Биба</t>
+  </si>
+  <si>
+    <t xml:space="preserve">УВ3463</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12:00-18:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Боба</t>
+  </si>
+  <si>
+    <t xml:space="preserve">КК2111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18:00-00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Пупа</t>
+  </si>
+  <si>
+    <t xml:space="preserve">МН3422</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00:00-06:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Лупа</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Модель</t>
+  </si>
+  <si>
     <t xml:space="preserve">Маршрут</t>
   </si>
   <si>
-    <t xml:space="preserve">Водитель</t>
-  </si>
-  <si>
     <t xml:space="preserve">Кондуктор</t>
   </si>
   <si>
-    <t xml:space="preserve">ID Автобуса</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Номер</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Модель</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID Смены</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Время</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID Водителя</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ФИО</t>
-  </si>
-  <si>
-    <t xml:space="preserve">АВ2453</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06:00-12:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Биба</t>
-  </si>
-  <si>
-    <t xml:space="preserve">УВ3463</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12:00-18:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Боба</t>
-  </si>
-  <si>
-    <t xml:space="preserve">КК2111</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18:00-00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Пупа</t>
-  </si>
-  <si>
-    <t xml:space="preserve">МН3422</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00:00-06:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Лупа</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID Модели</t>
-  </si>
-  <si>
     <t xml:space="preserve">Наименование</t>
   </si>
   <si>
-    <t xml:space="preserve">ID Маршрута</t>
-  </si>
-  <si>
     <t xml:space="preserve">Номер маршрута</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID Кондуктор</t>
   </si>
   <si>
     <t xml:space="preserve">ВАЗ</t>
@@ -244,7 +244,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -257,18 +257,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -289,19 +289,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -385,10 +373,10 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.59"/>
@@ -410,175 +398,175 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="C3" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="D3" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="E3" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F3" s="5" t="n">
+      <c r="A3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="E3" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C4" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="D4" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="E4" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="F4" s="5" t="n">
+      <c r="A4" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" s="4" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C5" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D5" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E5" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="F5" s="5" t="n">
+      <c r="A5" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="F5" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="C6" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F6" s="5" t="n">
+      <c r="A6" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="F6" s="4" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="n">
+      <c r="A7" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D7" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F7" s="5" t="n">
+      <c r="B7" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="F7" s="4" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
-        <v>2</v>
+      <c r="A9" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="B9" s="6"/>
-      <c r="E9" s="3" t="s">
-        <v>3</v>
+      <c r="E9" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="F9" s="6"/>
-      <c r="H9" s="3" t="s">
-        <v>5</v>
+      <c r="H9" s="5" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="I10" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="n">
+      <c r="A11" s="3" t="n">
         <v>1</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E11" s="4" t="n">
+      <c r="C11" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" s="3" t="n">
         <v>1</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="4" t="n">
+      <c r="H11" s="3" t="n">
         <v>1</v>
       </c>
       <c r="I11" s="8" t="s">
@@ -586,22 +574,22 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="n">
+      <c r="A12" s="3" t="n">
         <v>2</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E12" s="4" t="n">
+      <c r="C12" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3" t="n">
         <v>2</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="4" t="n">
+      <c r="H12" s="3" t="n">
         <v>2</v>
       </c>
       <c r="I12" s="8" t="s">
@@ -609,22 +597,22 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="n">
+      <c r="A13" s="3" t="n">
         <v>3</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="E13" s="4" t="n">
+      <c r="C13" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E13" s="3" t="n">
         <v>3</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="H13" s="4" t="n">
+      <c r="H13" s="3" t="n">
         <v>3</v>
       </c>
       <c r="I13" s="8" t="s">
@@ -632,22 +620,22 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="n">
+      <c r="A14" s="3" t="n">
         <v>4</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="E14" s="4" t="n">
+      <c r="C14" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E14" s="3" t="n">
         <v>4</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H14" s="4" t="n">
+      <c r="H14" s="3" t="n">
         <v>4</v>
       </c>
       <c r="I14" s="8" t="s">
@@ -656,66 +644,66 @@
       <c r="M14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="11"/>
+      <c r="A15" s="6"/>
       <c r="B15" s="10"/>
-      <c r="J15" s="11"/>
+      <c r="J15" s="6"/>
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>6</v>
+      <c r="A16" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G17" s="12"/>
+        <v>30</v>
+      </c>
+      <c r="G17" s="11"/>
       <c r="H17" s="2" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="I17" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="n">
+      <c r="A18" s="3" t="n">
         <v>1</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="4" t="n">
+      <c r="E18" s="3" t="n">
         <v>1</v>
       </c>
       <c r="F18" s="8" t="n">
         <v>14</v>
       </c>
-      <c r="G18" s="14"/>
-      <c r="H18" s="4" t="n">
+      <c r="G18" s="10"/>
+      <c r="H18" s="3" t="n">
         <v>1</v>
       </c>
       <c r="I18" s="8" t="s">
@@ -727,20 +715,20 @@
       <c r="M18" s="10"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4" t="n">
+      <c r="A19" s="3" t="n">
         <v>2</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="4" t="n">
+      <c r="E19" s="3" t="n">
         <v>2</v>
       </c>
       <c r="F19" s="8" t="n">
         <v>200</v>
       </c>
-      <c r="G19" s="14"/>
-      <c r="H19" s="4" t="n">
+      <c r="G19" s="10"/>
+      <c r="H19" s="3" t="n">
         <v>2</v>
       </c>
       <c r="I19" s="8" t="s">
@@ -750,14 +738,14 @@
       <c r="K19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E20" s="4" t="n">
+      <c r="E20" s="3" t="n">
         <v>3</v>
       </c>
       <c r="F20" s="8" t="n">
         <v>45</v>
       </c>
-      <c r="G20" s="14"/>
-      <c r="H20" s="4" t="n">
+      <c r="G20" s="10"/>
+      <c r="H20" s="3" t="n">
         <v>3</v>
       </c>
       <c r="I20" s="8" t="s">
@@ -767,13 +755,13 @@
       <c r="K20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E21" s="4" t="n">
+      <c r="E21" s="3" t="n">
         <v>4</v>
       </c>
       <c r="F21" s="8" t="n">
         <v>402</v>
       </c>
-      <c r="G21" s="14"/>
+      <c r="G21" s="10"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>